<commit_message>
added test data for cms1500 claim
</commit_message>
<xml_diff>
--- a/testData/AlphaPlusTestData.xlsx
+++ b/testData/AlphaPlusTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>testName</t>
   </si>
@@ -143,6 +143,51 @@
     <t>generatedLogin</t>
   </si>
   <si>
+    <t>patientid</t>
+  </si>
+  <si>
+    <t>patientSigndate</t>
+  </si>
+  <si>
+    <t>diagnosisCode</t>
+  </si>
+  <si>
+    <t>providerID</t>
+  </si>
+  <si>
+    <t>serviceFromDate</t>
+  </si>
+  <si>
+    <t>serviceToDate</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>procCode</t>
+  </si>
+  <si>
+    <t>serviceAmt</t>
+  </si>
+  <si>
+    <t>dayunits</t>
+  </si>
+  <si>
+    <t>diagnosispointer</t>
+  </si>
+  <si>
+    <t>renderingtaxonomyCode</t>
+  </si>
+  <si>
+    <t>physiciansigndate</t>
+  </si>
+  <si>
+    <t>sitephno</t>
+  </si>
+  <si>
+    <t>billingTaxonomyCode</t>
+  </si>
+  <si>
     <t>newPatientEnrollment</t>
   </si>
   <si>
@@ -228,6 +273,33 @@
   </si>
   <si>
     <t>tLgn77415579</t>
+  </si>
+  <si>
+    <t>createCMS1500Claim</t>
+  </si>
+  <si>
+    <t>07/13/2023</t>
+  </si>
+  <si>
+    <t>F70        *Mild intellectual disabilities</t>
+  </si>
+  <si>
+    <t>Group Home</t>
+  </si>
+  <si>
+    <t>YP770</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>251S00000X</t>
+  </si>
+  <si>
+    <t>08/16/2023</t>
+  </si>
+  <si>
+    <t>243-864-7452</t>
   </si>
   <si>
     <t>username</t>
@@ -252,11 +324,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -859,10 +932,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1183,15 +1257,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP3"/>
+  <dimension ref="A1:BE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="AZ6" sqref="AZ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="18.5904761904762" customWidth="1"/>
+    <col min="1" max="1" width="26.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="10.2952380952381" customWidth="1"/>
     <col min="3" max="3" width="13.5238095238095" customWidth="1"/>
     <col min="5" max="5" width="9.64761904761905" customWidth="1"/>
@@ -1219,9 +1293,24 @@
     <col min="39" max="39" width="23.7142857142857" customWidth="1"/>
     <col min="40" max="40" width="24.5714285714286" customWidth="1"/>
     <col min="42" max="42" width="16.8571428571429" customWidth="1"/>
+    <col min="43" max="43" width="13.7142857142857" customWidth="1"/>
+    <col min="44" max="44" width="16.8571428571429" customWidth="1"/>
+    <col min="45" max="45" width="15.5714285714286" customWidth="1"/>
+    <col min="46" max="46" width="15" customWidth="1"/>
+    <col min="47" max="47" width="18" customWidth="1"/>
+    <col min="48" max="48" width="11.1428571428571"/>
+    <col min="49" max="49" width="16.4285714285714" customWidth="1"/>
+    <col min="50" max="50" width="13.1428571428571" customWidth="1"/>
+    <col min="51" max="51" width="13.7142857142857" customWidth="1"/>
+    <col min="52" max="52" width="13.1428571428571" customWidth="1"/>
+    <col min="53" max="53" width="17.8571428571429" customWidth="1"/>
+    <col min="54" max="54" width="29.7142857142857" customWidth="1"/>
+    <col min="55" max="55" width="13.4285714285714" customWidth="1"/>
+    <col min="56" max="56" width="14.5714285714286" customWidth="1"/>
+    <col min="57" max="57" width="21.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:57">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1347,47 +1436,92 @@
       </c>
       <c r="AP1" t="s">
         <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:42">
       <c r="A2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="K2">
         <v>28269</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="N2">
         <v>3</v>
@@ -1396,28 +1530,28 @@
         <v>90000</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="X2"/>
       <c r="Y2"/>
@@ -1441,34 +1575,34 @@
     </row>
     <row r="3" spans="1:42">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="X3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="Y3" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="Z3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="AA3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="AB3">
         <v>1</v>
       </c>
       <c r="AC3" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="AD3" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="AE3" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="AG3">
         <v>8763612300</v>
@@ -1477,7 +1611,57 @@
         <v>21503</v>
       </c>
       <c r="AP3" t="s">
-        <v>70</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ4">
+        <v>37</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT4">
+        <v>1794</v>
+      </c>
+      <c r="AU4" s="3">
+        <v>44934</v>
+      </c>
+      <c r="AV4" s="3">
+        <v>44934</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY4">
+        <v>100</v>
+      </c>
+      <c r="AZ4">
+        <v>1</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>91</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>92</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>94</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1503,26 +1687,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added changes to get attribute values
</commit_message>
<xml_diff>
--- a/testData/AlphaPlusTestData.xlsx
+++ b/testData/AlphaPlusTestData.xlsx
@@ -305,10 +305,10 @@
     <t>243-864-7452</t>
   </si>
   <si>
-    <t>incomingFile837P</t>
-  </si>
-  <si>
-    <t>SingleClaimIncoming837p.jci</t>
+    <t>EDIincomingFile837PTest</t>
+  </si>
+  <si>
+    <t>Singleclaimediincoming837P.jci</t>
   </si>
   <si>
     <t>username</t>
@@ -1268,8 +1268,8 @@
   <sheetPr/>
   <dimension ref="A1:BF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BD8" sqref="BD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>

</xml_diff>

<commit_message>
added codes for cms1500 create save update and view
</commit_message>
<xml_diff>
--- a/testData/AlphaPlusTestData.xlsx
+++ b/testData/AlphaPlusTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="116">
   <si>
     <t>testName</t>
   </si>
@@ -191,6 +191,9 @@
     <t>EDIfileName</t>
   </si>
   <si>
+    <t>myMCSNumber</t>
+  </si>
+  <si>
     <t>newPatientEnrollment</t>
   </si>
   <si>
@@ -308,7 +311,94 @@
     <t>EDIincomingFile837PTest</t>
   </si>
   <si>
-    <t>Singleclaimediincoming837P.jci</t>
+    <t>Singleclaimediincoming837PEDI.jci</t>
+  </si>
+  <si>
+    <t>updateSaveCMS1500Claim</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>08/29/2023</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F30.11     Manic episode without psychotic symptoms, mild</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Office</t>
+    </r>
+  </si>
+  <si>
+    <t>6286</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>193200000X</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>865-437-8920</t>
+    </r>
+  </si>
+  <si>
+    <t>createSaveCMS1500Claim</t>
+  </si>
+  <si>
+    <t>updateSubmitCMS1500Claim</t>
+  </si>
+  <si>
+    <t>viewCMS1500Claim</t>
   </si>
   <si>
     <t>username</t>
@@ -941,12 +1031,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,15 +1365,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BF5"/>
+  <dimension ref="A1:BG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="30.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="10.2952380952381" customWidth="1"/>
     <col min="3" max="3" width="13.5238095238095" customWidth="1"/>
     <col min="5" max="5" width="9.64761904761905" customWidth="1"/>
@@ -1304,7 +1403,7 @@
     <col min="42" max="42" width="16.8571428571429" customWidth="1"/>
     <col min="43" max="43" width="13.7142857142857" customWidth="1"/>
     <col min="44" max="44" width="16.8571428571429" customWidth="1"/>
-    <col min="45" max="45" width="15.5714285714286" customWidth="1"/>
+    <col min="45" max="45" width="61.5714285714286" customWidth="1"/>
     <col min="46" max="46" width="15" customWidth="1"/>
     <col min="47" max="47" width="18" customWidth="1"/>
     <col min="48" max="48" width="11.1428571428571"/>
@@ -1317,10 +1416,11 @@
     <col min="55" max="55" width="13.4285714285714" customWidth="1"/>
     <col min="56" max="56" width="14.5714285714286" customWidth="1"/>
     <col min="57" max="57" width="21.5714285714286" customWidth="1"/>
-    <col min="58" max="58" width="31.1428571428571" customWidth="1"/>
+    <col min="58" max="58" width="35.2857142857143" customWidth="1"/>
+    <col min="59" max="59" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:59">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1494,47 +1594,50 @@
       </c>
       <c r="BF1" t="s">
         <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:42">
       <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K2">
         <v>28269</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N2">
         <v>3</v>
@@ -1543,28 +1646,28 @@
         <v>90000</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="X2"/>
       <c r="Y2"/>
@@ -1588,34 +1691,34 @@
     </row>
     <row r="3" spans="1:42">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="X3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Y3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AA3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AB3">
         <v>1</v>
       </c>
       <c r="AC3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AD3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AE3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AG3">
         <v>8763612300</v>
@@ -1624,21 +1727,21 @@
         <v>21503</v>
       </c>
       <c r="AP3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:57">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AQ4">
         <v>37</v>
       </c>
       <c r="AR4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AS4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AT4">
         <v>1794</v>
@@ -1650,10 +1753,10 @@
         <v>44934</v>
       </c>
       <c r="AW4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AX4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AY4">
         <v>100</v>
@@ -1662,27 +1765,183 @@
         <v>1</v>
       </c>
       <c r="BA4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BB4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="BC4" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE4" t="s">
         <v>94</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>95</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:58">
       <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" ht="13" customHeight="1" spans="1:59">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AS6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="5">
+        <v>44932</v>
+      </c>
+      <c r="AV6" s="5">
+        <v>44932</v>
+      </c>
+      <c r="AW6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX6" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY6" s="4">
+        <v>54</v>
+      </c>
+      <c r="AZ6" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="BB6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BE6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="BG6">
+        <v>250625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:57">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AQ7">
+        <v>37</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT7">
+        <v>1794</v>
+      </c>
+      <c r="AU7" s="3">
+        <v>44934</v>
+      </c>
+      <c r="AV7" s="3">
+        <v>44934</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY7">
+        <v>100</v>
+      </c>
+      <c r="AZ7">
+        <v>1</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>94</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD7" t="s">
         <v>96</v>
       </c>
-      <c r="BF5" t="s">
-        <v>97</v>
+      <c r="BE7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT8">
+        <v>1794</v>
+      </c>
+      <c r="AU8" s="3">
+        <v>44934</v>
+      </c>
+      <c r="AV8" s="3">
+        <v>44934</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY8">
+        <v>100</v>
+      </c>
+      <c r="AZ8">
+        <v>1</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>94</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG8">
+        <v>250635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="BG9">
+        <v>250625</v>
       </c>
     </row>
   </sheetData>
@@ -1708,26 +1967,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>